<commit_message>
Updated code and protocol
</commit_message>
<xml_diff>
--- a/cp1/tostogan_fb-01_novak_fb-01_cp1/bigram1.xlsx
+++ b/cp1/tostogan_fb-01_novak_fb-01_cp1/bigram1.xlsx
@@ -582,85 +582,85 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.0004209745005774551</v>
+        <v>0.0005274384784859596</v>
       </c>
       <c r="C2">
-        <v>0.001786372058371438</v>
+        <v>0.001017897875454454</v>
       </c>
       <c r="D2">
-        <v>0.005821634211932965</v>
+        <v>0.005772629251621241</v>
       </c>
       <c r="E2">
-        <v>0.001514954288262289</v>
+        <v>0.001669897470630824</v>
       </c>
       <c r="F2">
-        <v>0.003162847892496407</v>
+        <v>0.003026445882087333</v>
       </c>
       <c r="G2">
-        <v>0.001415249801283418</v>
+        <v>0.002238207565530825</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.001542649979089753</v>
+        <v>0.002310219461117469</v>
       </c>
       <c r="J2">
-        <v>0.004096192673381949</v>
+        <v>0.004118301920576718</v>
       </c>
       <c r="K2">
-        <v>0.001478949890186586</v>
+        <v>0.001592046772699317</v>
       </c>
       <c r="L2">
-        <v>0.0009499621953820205</v>
+        <v>0.0009166919681434944</v>
       </c>
       <c r="M2">
-        <v>0.005098776681336151</v>
+        <v>0.00758849678087364</v>
       </c>
       <c r="N2">
-        <v>0.01017539681001033</v>
+        <v>0.00957952838047193</v>
       </c>
       <c r="O2">
-        <v>0.004830128480309749</v>
+        <v>0.004680773213131856</v>
       </c>
       <c r="P2">
-        <v>0.007746484724441724</v>
+        <v>0.005918599310242816</v>
       </c>
       <c r="Q2">
-        <v>0.000999814438871456</v>
+        <v>0.001158029131731166</v>
       </c>
       <c r="R2">
-        <v>0.003841392317769278</v>
+        <v>0.002559341694498291</v>
       </c>
       <c r="S2">
-        <v>0.005048924437846715</v>
+        <v>0.002656655066912675</v>
       </c>
       <c r="T2">
-        <v>0.006644196229508651</v>
+        <v>0.007781177258254121</v>
       </c>
       <c r="U2">
-        <v>0.007375362467353704</v>
+        <v>0.005513775680998981</v>
       </c>
       <c r="V2">
-        <v>0.0006619270107763933</v>
+        <v>0.0005352235482791103</v>
       </c>
       <c r="W2">
-        <v>0.0005483746783837902</v>
+        <v>0.0002432834310359592</v>
       </c>
       <c r="X2">
-        <v>0.00172267196946827</v>
+        <v>0.001008166538213015</v>
       </c>
       <c r="Y2">
-        <v>0.0005317572638873117</v>
+        <v>6.617309324178092E-05</v>
       </c>
       <c r="Z2">
-        <v>0.001415249801283418</v>
+        <v>0.001687413877665413</v>
       </c>
       <c r="AA2">
-        <v>0.001168758152918987</v>
+        <v>0.001158029131731166</v>
       </c>
       <c r="AB2">
-        <v>0.0003351178590123163</v>
+        <v>0.0002082506169667811</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -672,13 +672,13 @@
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>0.0003074221681848521</v>
+        <v>0.0003483818732434936</v>
       </c>
       <c r="AG2">
-        <v>0.0007699402050035035</v>
+        <v>0.001152190329386303</v>
       </c>
       <c r="AH2">
-        <v>0.002697560286595009</v>
+        <v>0.002598267043464044</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -686,103 +686,103 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.001246306087235887</v>
+        <v>0.0006578383975212338</v>
       </c>
       <c r="C3">
-        <v>1.384784541373208E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="D3">
-        <v>6.646965798591397E-05</v>
+        <v>6.033429089691789E-05</v>
       </c>
       <c r="E3">
-        <v>5.539138165492831E-06</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="F3">
-        <v>1.938698357922491E-05</v>
+        <v>2.335520937945209E-05</v>
       </c>
       <c r="G3">
-        <v>0.00253415571071297</v>
+        <v>0.002804571392982538</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2.215655266197132E-05</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="J3">
-        <v>1.938698357922491E-05</v>
+        <v>2.140894193116441E-05</v>
       </c>
       <c r="K3">
-        <v>0.001116136340346805</v>
+        <v>0.0008135397933842477</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>9.416534881337813E-05</v>
+        <v>0.0001303999190352742</v>
       </c>
       <c r="N3">
-        <v>0.001243536518153141</v>
+        <v>0.0007434741652458915</v>
       </c>
       <c r="O3">
-        <v>2.769569082746415E-05</v>
+        <v>6.617309324178092E-05</v>
       </c>
       <c r="P3">
-        <v>0.0002963438918538664</v>
+        <v>0.0003308654662089046</v>
       </c>
       <c r="Q3">
-        <v>0.00238736854932741</v>
+        <v>0.002228476228289387</v>
       </c>
       <c r="R3">
-        <v>3.046525991021057E-05</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="S3">
-        <v>0.001642354466068624</v>
+        <v>0.001080178433799659</v>
       </c>
       <c r="T3">
-        <v>0.0002215655266197132</v>
+        <v>0.0001926804773804797</v>
       </c>
       <c r="U3">
-        <v>1.938698357922491E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="V3">
-        <v>0.001185375567415466</v>
+        <v>0.001448022981526029</v>
       </c>
       <c r="W3">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>2.769569082746415E-05</v>
+        <v>4.671041875890417E-05</v>
       </c>
       <c r="Y3">
-        <v>8.308707248239246E-06</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <v>3.877396715844982E-05</v>
+        <v>2.724774427602743E-05</v>
       </c>
       <c r="AA3">
-        <v>3.60043980757034E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="AB3">
-        <v>0.0003185004445158378</v>
+        <v>0.0002432834310359592</v>
       </c>
       <c r="AC3">
-        <v>0.000180021990378517</v>
+        <v>0.0002004655471736304</v>
       </c>
       <c r="AD3">
-        <v>0.003101917372675985</v>
+        <v>0.004873453690512335</v>
       </c>
       <c r="AE3">
-        <v>0.0003240395826813306</v>
+        <v>3.69790815174658E-05</v>
       </c>
       <c r="AF3">
-        <v>2.769569082746415E-05</v>
+        <v>0.0001284536515869865</v>
       </c>
       <c r="AG3">
-        <v>9.139577973063171E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="AH3">
-        <v>0.0002658786319436559</v>
+        <v>0.0006675697347626722</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -790,103 +790,103 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.007862806625917073</v>
+        <v>0.007107768721146585</v>
       </c>
       <c r="C4">
-        <v>0.0003074221681848521</v>
+        <v>0.0001965730122770551</v>
       </c>
       <c r="D4">
-        <v>0.0005899182146249866</v>
+        <v>0.0004262325711750006</v>
       </c>
       <c r="E4">
-        <v>0.0005788399382940008</v>
+        <v>0.0004573728503476034</v>
       </c>
       <c r="F4">
-        <v>0.0007477836523415322</v>
+        <v>0.001214470887731509</v>
       </c>
       <c r="G4">
-        <v>0.006566648295191751</v>
+        <v>0.006514157149418845</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>9.693491789612454E-05</v>
+        <v>5.060295365547952E-05</v>
       </c>
       <c r="J4">
-        <v>0.0005179094184735797</v>
+        <v>0.000626698118348631</v>
       </c>
       <c r="K4">
-        <v>0.004248518972933001</v>
+        <v>0.004046290024990074</v>
       </c>
       <c r="L4">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>0.001091210218602088</v>
+        <v>0.0005663638274517131</v>
       </c>
       <c r="N4">
-        <v>0.001077362373188356</v>
+        <v>0.001175545538765755</v>
       </c>
       <c r="O4">
-        <v>0.0004791354513151299</v>
+        <v>0.0002724774427602743</v>
       </c>
       <c r="P4">
-        <v>0.001697745847723553</v>
+        <v>0.002534040217670551</v>
       </c>
       <c r="Q4">
-        <v>0.008184076639515658</v>
+        <v>0.007590443048321929</v>
       </c>
       <c r="R4">
-        <v>0.001080131942271102</v>
+        <v>0.00120473955049007</v>
       </c>
       <c r="S4">
-        <v>0.001099518925850327</v>
+        <v>0.0007434741652458915</v>
       </c>
       <c r="T4">
-        <v>0.003182234876075631</v>
+        <v>0.005186802749686651</v>
       </c>
       <c r="U4">
-        <v>0.001080131942271102</v>
+        <v>0.000710387618625001</v>
       </c>
       <c r="V4">
-        <v>0.001019201422450681</v>
+        <v>0.0007026025488318503</v>
       </c>
       <c r="W4">
-        <v>5.262181257218189E-05</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="X4">
-        <v>0.000180021990378517</v>
+        <v>7.395816303493161E-05</v>
       </c>
       <c r="Y4">
-        <v>0.0001357088850545744</v>
+        <v>4.281788386232883E-05</v>
       </c>
       <c r="Z4">
-        <v>0.000279726477357388</v>
+        <v>0.0003075102568294525</v>
       </c>
       <c r="AA4">
-        <v>0.001152140738422509</v>
+        <v>0.0008544114097982889</v>
       </c>
       <c r="AB4">
-        <v>2.492612174471774E-05</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="AC4">
-        <v>5.539138165492831E-06</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="AD4">
-        <v>0.003348409021040416</v>
+        <v>0.003764081244988361</v>
       </c>
       <c r="AE4">
-        <v>0.0001218610396408423</v>
+        <v>0.0001498625935181509</v>
       </c>
       <c r="AF4">
-        <v>0.0001634045758820385</v>
+        <v>0.0004184475013818499</v>
       </c>
       <c r="AG4">
-        <v>1.661741449647849E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="AH4">
-        <v>0.0003849701025017518</v>
+        <v>0.0002160356867599318</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -894,82 +894,82 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.001894385252598548</v>
+        <v>0.001379903620835961</v>
       </c>
       <c r="C5">
-        <v>3.323482899295698E-05</v>
+        <v>3.892534896575348E-05</v>
       </c>
       <c r="D5">
-        <v>6.923922706866039E-05</v>
+        <v>0.0001187223143455481</v>
       </c>
       <c r="E5">
-        <v>1.661741449647849E-05</v>
+        <v>2.724774427602743E-05</v>
       </c>
       <c r="F5">
-        <v>0.0008641055538168817</v>
+        <v>0.001366279748697947</v>
       </c>
       <c r="G5">
-        <v>0.000473596313149637</v>
+        <v>0.0009770262590404124</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>8.308707248239246E-06</v>
+        <v>7.785069793150696E-06</v>
       </c>
       <c r="J5">
-        <v>3.046525991021057E-05</v>
+        <v>7.201189558664393E-05</v>
       </c>
       <c r="K5">
-        <v>0.0009970448697887095</v>
+        <v>0.0006364294555900693</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0.0001634045758820385</v>
+        <v>0.0001050984422075344</v>
       </c>
       <c r="N5">
-        <v>0.001276771347146098</v>
+        <v>0.001967676390218838</v>
       </c>
       <c r="O5">
-        <v>3.60043980757034E-05</v>
+        <v>5.060295365547952E-05</v>
       </c>
       <c r="P5">
-        <v>0.0002852656155228808</v>
+        <v>0.0003308654662089046</v>
       </c>
       <c r="Q5">
-        <v>0.008447185702376568</v>
+        <v>0.01000381468419864</v>
       </c>
       <c r="R5">
-        <v>7.477836523415322E-05</v>
+        <v>0.0001654327331044523</v>
       </c>
       <c r="S5">
-        <v>0.001650663173316864</v>
+        <v>0.0005760951646931515</v>
       </c>
       <c r="T5">
-        <v>0.0001080131942271102</v>
+        <v>0.0001245611166904111</v>
       </c>
       <c r="U5">
-        <v>1.107827633098566E-05</v>
+        <v>3.69790815174658E-05</v>
       </c>
       <c r="V5">
-        <v>0.0008142533103274462</v>
+        <v>0.0005469011529688364</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="X5">
-        <v>2.769569082746416E-06</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="Z5">
-        <v>2.492612174471774E-05</v>
+        <v>5.644175600034255E-05</v>
       </c>
       <c r="AA5">
-        <v>1.938698357922491E-05</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="AB5">
         <v>0</v>
@@ -981,16 +981,16 @@
         <v>0</v>
       </c>
       <c r="AE5">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AF5">
-        <v>1.938698357922491E-05</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="AG5">
         <v>0</v>
       </c>
       <c r="AH5">
-        <v>2.769569082746416E-06</v>
+        <v>2.724774427602743E-05</v>
       </c>
     </row>
     <row r="6" spans="1:34">
@@ -998,103 +998,103 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.00528433780988016</v>
+        <v>0.006535566091350009</v>
       </c>
       <c r="C6">
-        <v>0.0001080131942271102</v>
+        <v>3.69790815174658E-05</v>
       </c>
       <c r="D6">
-        <v>0.001454023768441868</v>
+        <v>0.0008738740842811656</v>
       </c>
       <c r="E6">
-        <v>6.370008890316756E-05</v>
+        <v>2.724774427602743E-05</v>
       </c>
       <c r="F6">
-        <v>0.0001052436251443638</v>
+        <v>3.69790815174658E-05</v>
       </c>
       <c r="G6">
-        <v>0.005669307912381912</v>
+        <v>0.00522962063354898</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>8.86262106478853E-05</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="J6">
-        <v>8.308707248239247E-05</v>
+        <v>4.671041875890417E-05</v>
       </c>
       <c r="K6">
-        <v>0.002960669349455918</v>
+        <v>0.002705311753119867</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0.0004763658822323835</v>
+        <v>0.0004087161641404115</v>
       </c>
       <c r="N6">
-        <v>0.000720087961514068</v>
+        <v>0.0007084413511767133</v>
       </c>
       <c r="O6">
-        <v>0.0001661741449647849</v>
+        <v>4.865668620719185E-05</v>
       </c>
       <c r="P6">
-        <v>0.002151955177293965</v>
+        <v>0.002349144810083222</v>
       </c>
       <c r="Q6">
-        <v>0.004497780190380178</v>
+        <v>0.004599029980303773</v>
       </c>
       <c r="R6">
-        <v>0.0002880351846056272</v>
+        <v>0.0001479163260698632</v>
       </c>
       <c r="S6">
-        <v>0.00113552332392603</v>
+        <v>0.001868416750356167</v>
       </c>
       <c r="T6">
-        <v>0.0007145488233485752</v>
+        <v>0.0004223400362784252</v>
       </c>
       <c r="U6">
-        <v>0.0001744828522130242</v>
+        <v>0.0002938863846914387</v>
       </c>
       <c r="V6">
-        <v>0.001783602489288692</v>
+        <v>0.001792512319872948</v>
       </c>
       <c r="W6">
-        <v>5.539138165492831E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="X6">
-        <v>4.985224348943548E-05</v>
+        <v>8.17432328280823E-05</v>
       </c>
       <c r="Y6">
-        <v>0.0004154353624119623</v>
+        <v>0.0003834146873126718</v>
       </c>
       <c r="Z6">
-        <v>8.308707248239247E-05</v>
+        <v>0.0001128835120006851</v>
       </c>
       <c r="AA6">
-        <v>8.585664156513888E-05</v>
+        <v>8.758203517294533E-05</v>
       </c>
       <c r="AB6">
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>4.431310532394265E-05</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="AD6">
-        <v>0.000720087961514068</v>
+        <v>0.000543008618072261</v>
       </c>
       <c r="AE6">
-        <v>0.0004431310532394265</v>
+        <v>0.00100427400331644</v>
       </c>
       <c r="AF6">
-        <v>8.308707248239246E-06</v>
+        <v>1.751640703458906E-05</v>
       </c>
       <c r="AG6">
-        <v>4.154353624119623E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="AH6">
-        <v>0.0003988179479154838</v>
+        <v>0.0003152953266226031</v>
       </c>
     </row>
     <row r="7" spans="1:34">
@@ -1102,85 +1102,85 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.0005151398493908332</v>
+        <v>0.0002316058263462332</v>
       </c>
       <c r="C7">
-        <v>0.001949776634253476</v>
+        <v>0.00255155662470514</v>
       </c>
       <c r="D7">
-        <v>0.004758119684158342</v>
+        <v>0.004914325306926376</v>
       </c>
       <c r="E7">
-        <v>0.003243165395896053</v>
+        <v>0.004324606270095212</v>
       </c>
       <c r="F7">
-        <v>0.004350993028994618</v>
+        <v>0.004466683793820212</v>
       </c>
       <c r="G7">
-        <v>0.00206332896664608</v>
+        <v>0.002319950798358907</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0.001340471436049265</v>
+        <v>0.001080178433799659</v>
       </c>
       <c r="J7">
-        <v>0.00206332896664608</v>
+        <v>0.002473705926773634</v>
       </c>
       <c r="K7">
-        <v>0.001163219014753494</v>
+        <v>0.001664058668285961</v>
       </c>
       <c r="L7">
-        <v>0.002564620970623181</v>
+        <v>0.002615783450498634</v>
       </c>
       <c r="M7">
-        <v>0.002636629766774588</v>
+        <v>0.002545717822360277</v>
       </c>
       <c r="N7">
-        <v>0.007090096851830823</v>
+        <v>0.006638718266109255</v>
       </c>
       <c r="O7">
-        <v>0.004495010621297433</v>
+        <v>0.006122957392313022</v>
       </c>
       <c r="P7">
-        <v>0.01030279698781666</v>
+        <v>0.01084265595441063</v>
       </c>
       <c r="Q7">
-        <v>0.001420788939448911</v>
+        <v>0.001669897470630824</v>
       </c>
       <c r="R7">
-        <v>0.00290527796780099</v>
+        <v>0.003921728908299663</v>
       </c>
       <c r="S7">
-        <v>0.008062215599874816</v>
+        <v>0.00763909973452912</v>
       </c>
       <c r="T7">
-        <v>0.007380901605519197</v>
+        <v>0.007434741652458914</v>
       </c>
       <c r="U7">
-        <v>0.006392165442978727</v>
+        <v>0.007607959455356517</v>
       </c>
       <c r="V7">
-        <v>0.0007588619286725178</v>
+        <v>0.0008719278168328779</v>
       </c>
       <c r="W7">
-        <v>0.0001634045758820385</v>
+        <v>0.0001128835120006851</v>
       </c>
       <c r="X7">
-        <v>0.0008031750339964605</v>
+        <v>0.0009478322473160972</v>
       </c>
       <c r="Y7">
-        <v>0.0006619270107763933</v>
+        <v>0.0005118683388996582</v>
       </c>
       <c r="Z7">
-        <v>0.001567576100834471</v>
+        <v>0.002148679262909592</v>
       </c>
       <c r="AA7">
-        <v>0.000866875122899628</v>
+        <v>0.001150244061938015</v>
       </c>
       <c r="AB7">
-        <v>0.0007588619286725178</v>
+        <v>0.00103736054993733</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -1192,13 +1192,13 @@
         <v>0</v>
       </c>
       <c r="AF7">
-        <v>0.0002104872502887276</v>
+        <v>0.0003620057453815074</v>
       </c>
       <c r="AG7">
-        <v>0.0001329393159718279</v>
+        <v>0.0002861013148982881</v>
       </c>
       <c r="AH7">
-        <v>0.0003295787208468234</v>
+        <v>0.0006481070602797955</v>
       </c>
     </row>
     <row r="8" spans="1:34">
@@ -1206,82 +1206,82 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>3.69790815174658E-05</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>5.060295365547952E-05</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>4.281788386232883E-05</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>2.335520937945209E-05</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>3.114027917260278E-05</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>2.140894193116441E-05</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>2.919401172431511E-05</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>3.114027917260278E-05</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>2.335520937945209E-05</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>6.617309324178092E-05</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>5.254922110376719E-05</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>5.254922110376719E-05</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>3.892534896575348E-05</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>4.087161641404115E-05</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="AB8">
         <v>0</v>
@@ -1296,13 +1296,13 @@
         <v>0</v>
       </c>
       <c r="AF8">
-        <v>0</v>
+        <v>0.0001498625935181509</v>
       </c>
       <c r="AG8">
         <v>0</v>
       </c>
       <c r="AH8">
-        <v>0</v>
+        <v>5.838802344863021E-06</v>
       </c>
     </row>
     <row r="9" spans="1:34">
@@ -1310,79 +1310,79 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.001495567304683064</v>
+        <v>0.001576476633113016</v>
       </c>
       <c r="C9">
-        <v>4.154353624119623E-05</v>
+        <v>6.811936069006858E-05</v>
       </c>
       <c r="D9">
-        <v>2.492612174471774E-05</v>
+        <v>3.308654662089046E-05</v>
       </c>
       <c r="E9">
-        <v>1.938698357922491E-05</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="F9">
-        <v>0.0009859665934577239</v>
+        <v>0.001014005340557878</v>
       </c>
       <c r="G9">
-        <v>0.003578283254908369</v>
+        <v>0.005838802344863022</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="I9">
-        <v>8.308707248239246E-06</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="J9">
-        <v>1.384784541373208E-05</v>
+        <v>1.751640703458906E-05</v>
       </c>
       <c r="K9">
-        <v>0.001589732653496442</v>
+        <v>0.001621240784423632</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0.0002049481121232348</v>
+        <v>7.590443048321929E-05</v>
       </c>
       <c r="N9">
-        <v>1.384784541373208E-05</v>
+        <v>3.114027917260278E-05</v>
       </c>
       <c r="O9">
-        <v>1.107827633098566E-05</v>
+        <v>1.167760468972604E-05</v>
       </c>
       <c r="P9">
-        <v>0.001038588406029906</v>
+        <v>0.0009964889335232891</v>
       </c>
       <c r="Q9">
-        <v>0.0001163219014753494</v>
+        <v>8.563576772465765E-05</v>
       </c>
       <c r="R9">
-        <v>1.384784541373208E-05</v>
+        <v>5.449548855205487E-05</v>
       </c>
       <c r="S9">
-        <v>5.539138165492831E-06</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="T9">
-        <v>5.816095073767472E-05</v>
+        <v>6.033429089691789E-05</v>
       </c>
       <c r="U9">
-        <v>1.661741449647849E-05</v>
+        <v>7.006562813835626E-05</v>
       </c>
       <c r="V9">
-        <v>0.0002520307865299238</v>
+        <v>0.0002530147682773976</v>
       </c>
       <c r="W9">
-        <v>5.539138165492831E-06</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>7.785069793150696E-06</v>
       </c>
       <c r="Y9">
-        <v>5.539138165492831E-06</v>
+        <v>0</v>
       </c>
       <c r="Z9">
-        <v>3.323482899295698E-05</v>
+        <v>2.530147682773976E-05</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -1397,16 +1397,16 @@
         <v>0</v>
       </c>
       <c r="AE9">
-        <v>3.60043980757034E-05</v>
+        <v>2.919401172431511E-05</v>
       </c>
       <c r="AF9">
-        <v>8.308707248239246E-06</v>
+        <v>2.919401172431511E-05</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="AH9">
-        <v>8.308707248239246E-06</v>
+        <v>1.557013958630139E-05</v>
       </c>
     </row>
     <row r="10" spans="1:34">
@@ -1414,103 +1414,103 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.005536368596410084</v>
+        <v>0.005673369611758569</v>
       </c>
       <c r="C10">
-        <v>0.0001717132831302778</v>
+        <v>0.0001751640703458907</v>
       </c>
       <c r="D10">
-        <v>0.001279540916228844</v>
+        <v>0.001282590248421577</v>
       </c>
       <c r="E10">
-        <v>0.0003074221681848521</v>
+        <v>0.0005021370016582198</v>
       </c>
       <c r="F10">
-        <v>0.001154910307505255</v>
+        <v>0.0007746144444184942</v>
       </c>
       <c r="G10">
-        <v>0.000673005287107379</v>
+        <v>0.0003269729313123292</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.0001412480232200672</v>
+        <v>6.228055834520557E-05</v>
       </c>
       <c r="J10">
-        <v>0.0001384784541373208</v>
+        <v>6.617309324178092E-05</v>
       </c>
       <c r="K10">
-        <v>0.0007754793431689963</v>
+        <v>0.0004982444667616445</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0.0002908047536883736</v>
+        <v>0.0002043580820702058</v>
       </c>
       <c r="N10">
-        <v>0.0002603394937781631</v>
+        <v>0.0002822087800017127</v>
       </c>
       <c r="O10">
-        <v>0.0004957528658116084</v>
+        <v>0.0003191878615191785</v>
       </c>
       <c r="P10">
-        <v>0.001747598091212988</v>
+        <v>0.002426995508014729</v>
       </c>
       <c r="Q10">
-        <v>0.001008123146119695</v>
+        <v>0.0006052891764174665</v>
       </c>
       <c r="R10">
-        <v>0.0002520307865299238</v>
+        <v>0.0002024118146219181</v>
       </c>
       <c r="S10">
-        <v>0.0003240395826813306</v>
+        <v>0.0002919401172431511</v>
       </c>
       <c r="T10">
-        <v>0.0002492612174471774</v>
+        <v>0.0001751640703458907</v>
       </c>
       <c r="U10">
-        <v>9.970448697887096E-05</v>
+        <v>8.758203517294533E-05</v>
       </c>
       <c r="V10">
-        <v>0.0004320527769084408</v>
+        <v>0.0003620057453815074</v>
       </c>
       <c r="W10">
-        <v>1.107827633098566E-05</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="X10">
-        <v>5.539138165492831E-06</v>
+        <v>7.785069793150696E-06</v>
       </c>
       <c r="Y10">
-        <v>2.215655266197132E-05</v>
+        <v>1.751640703458906E-05</v>
       </c>
       <c r="Z10">
-        <v>8.86262106478853E-05</v>
+        <v>5.838802344863021E-05</v>
       </c>
       <c r="AA10">
-        <v>3.60043980757034E-05</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="AB10">
         <v>0</v>
       </c>
       <c r="AC10">
-        <v>1.661741449647849E-05</v>
+        <v>3.892534896575348E-05</v>
       </c>
       <c r="AD10">
-        <v>0.0005539138165492831</v>
+        <v>0.0003795221524160964</v>
       </c>
       <c r="AE10">
-        <v>9.139577973063171E-05</v>
+        <v>0.001504464737526372</v>
       </c>
       <c r="AF10">
-        <v>2.492612174471774E-05</v>
+        <v>4.281788386232883E-05</v>
       </c>
       <c r="AG10">
-        <v>2.769569082746416E-06</v>
+        <v>0.0001771103377941783</v>
       </c>
       <c r="AH10">
-        <v>0.0002880351846056272</v>
+        <v>0.0006773010720041105</v>
       </c>
     </row>
     <row r="11" spans="1:34">
@@ -1518,85 +1518,85 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.0008641055538168817</v>
+        <v>0.0002958326521397264</v>
       </c>
       <c r="C11">
-        <v>0.001127214616677791</v>
+        <v>0.001658219865941098</v>
       </c>
       <c r="D11">
-        <v>0.004478393206800954</v>
+        <v>0.004959089458236993</v>
       </c>
       <c r="E11">
-        <v>0.001312775745221801</v>
+        <v>0.0008933367587640424</v>
       </c>
       <c r="F11">
-        <v>0.002708638562925994</v>
+        <v>0.002950541451604114</v>
       </c>
       <c r="G11">
-        <v>0.003004982454779861</v>
+        <v>0.002382231356704113</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.0005096007112253405</v>
+        <v>0.0004067698966921238</v>
       </c>
       <c r="J11">
-        <v>0.003317943761130206</v>
+        <v>0.002845443009396579</v>
       </c>
       <c r="K11">
-        <v>0.002520307865299238</v>
+        <v>0.001704930284700002</v>
       </c>
       <c r="L11">
-        <v>0.00209379422655629</v>
+        <v>0.001167760468972604</v>
       </c>
       <c r="M11">
-        <v>0.004542093295704121</v>
+        <v>0.002699472950775004</v>
       </c>
       <c r="N11">
-        <v>0.005816095073767472</v>
+        <v>0.006808043534110284</v>
       </c>
       <c r="O11">
-        <v>0.003650292051059776</v>
+        <v>0.003402075499606854</v>
       </c>
       <c r="P11">
-        <v>0.006680200627584354</v>
+        <v>0.00593222318238083</v>
       </c>
       <c r="Q11">
-        <v>0.001966394048749955</v>
+        <v>0.00165627359849281</v>
       </c>
       <c r="R11">
-        <v>0.003353948159205909</v>
+        <v>0.002802625125534251</v>
       </c>
       <c r="S11">
-        <v>0.002304281476845018</v>
+        <v>0.0008446800725568505</v>
       </c>
       <c r="T11">
-        <v>0.006115208534704085</v>
+        <v>0.004513394212579116</v>
       </c>
       <c r="U11">
-        <v>0.006131825949200564</v>
+        <v>0.006037321624588365</v>
       </c>
       <c r="V11">
-        <v>0.0005539138165492831</v>
+        <v>0.0005566324902102748</v>
       </c>
       <c r="W11">
-        <v>0.0002991134609366129</v>
+        <v>0.0001634864656561646</v>
       </c>
       <c r="X11">
-        <v>0.002019015861322137</v>
+        <v>0.0016737900055274</v>
       </c>
       <c r="Y11">
-        <v>0.001301697468890815</v>
+        <v>0.0009711874566955493</v>
       </c>
       <c r="Z11">
-        <v>0.003279169793971756</v>
+        <v>0.002643031194774661</v>
       </c>
       <c r="AA11">
-        <v>0.0006813139943556183</v>
+        <v>0.0007882383165565079</v>
       </c>
       <c r="AB11">
-        <v>0.0004015875169982303</v>
+        <v>0.00016737900055274</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -1608,13 +1608,13 @@
         <v>0</v>
       </c>
       <c r="AF11">
-        <v>0.0002381829411161917</v>
+        <v>0.0002354983612428085</v>
       </c>
       <c r="AG11">
-        <v>0.0004791354513151299</v>
+        <v>0.0003133490591743155</v>
       </c>
       <c r="AH11">
-        <v>0.001935928788839744</v>
+        <v>0.001671843738079112</v>
       </c>
     </row>
     <row r="12" spans="1:34">
@@ -1622,85 +1622,85 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.0002437220792816846</v>
+        <v>0.0001440237911732879</v>
       </c>
       <c r="C12">
-        <v>0.0003877396715844981</v>
+        <v>0.0002218744891047948</v>
       </c>
       <c r="D12">
-        <v>0.0007616314977552642</v>
+        <v>0.0006208593160037679</v>
       </c>
       <c r="E12">
-        <v>0.0004403614841566801</v>
+        <v>0.0002179819542082195</v>
       </c>
       <c r="F12">
-        <v>0.0006702357180246325</v>
+        <v>0.0006695160022109598</v>
       </c>
       <c r="G12">
-        <v>0.0001301697468890815</v>
+        <v>8.758203517294533E-05</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.0001938698357922491</v>
+        <v>0.0001634864656561646</v>
       </c>
       <c r="J12">
-        <v>0.0003074221681848521</v>
+        <v>0.0001498625935181509</v>
       </c>
       <c r="K12">
-        <v>0.0006646965798591398</v>
+        <v>0.0006870324092455489</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>0.00102751012969892</v>
+        <v>0.0005391160831756857</v>
       </c>
       <c r="N12">
-        <v>0.0003074221681848521</v>
+        <v>0.0001537551284147262</v>
       </c>
       <c r="O12">
-        <v>0.0005096007112253405</v>
+        <v>0.0004087161641404115</v>
       </c>
       <c r="P12">
-        <v>0.001024740560616174</v>
+        <v>0.001089909771041097</v>
       </c>
       <c r="Q12">
-        <v>0.0005151398493908332</v>
+        <v>0.0003289191987606169</v>
       </c>
       <c r="R12">
-        <v>0.001177066860167227</v>
+        <v>0.0007570980373839051</v>
       </c>
       <c r="S12">
-        <v>0.0004071266551637231</v>
+        <v>0.0002607998380705483</v>
       </c>
       <c r="T12">
-        <v>0.001678358864144328</v>
+        <v>0.001374064818491098</v>
       </c>
       <c r="U12">
-        <v>0.00077270977408625</v>
+        <v>0.000722065223314727</v>
       </c>
       <c r="V12">
-        <v>0.0001689437140475313</v>
+        <v>0.0001440237911732879</v>
       </c>
       <c r="W12">
-        <v>0.0001080131942271102</v>
+        <v>7.979696537979462E-05</v>
       </c>
       <c r="X12">
-        <v>9.416534881337813E-05</v>
+        <v>4.865668620719185E-05</v>
       </c>
       <c r="Y12">
-        <v>9.970448697887096E-05</v>
+        <v>0.000101205907310959</v>
       </c>
       <c r="Z12">
-        <v>0.0004126657933292159</v>
+        <v>0.000543008618072261</v>
       </c>
       <c r="AA12">
-        <v>0.0002187959575369668</v>
+        <v>0.0003114027917260278</v>
       </c>
       <c r="AB12">
-        <v>8.308707248239246E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -1712,13 +1712,13 @@
         <v>0</v>
       </c>
       <c r="AF12">
-        <v>7.754793431689964E-05</v>
+        <v>8.17432328280823E-05</v>
       </c>
       <c r="AG12">
-        <v>1.661741449647849E-05</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="AH12">
-        <v>7.20087961514068E-05</v>
+        <v>8.368950027636998E-05</v>
       </c>
     </row>
     <row r="13" spans="1:34">
@@ -1726,82 +1726,82 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.007752023862607217</v>
+        <v>0.007528162489976723</v>
       </c>
       <c r="C13">
-        <v>0.0002215655266197132</v>
+        <v>0.0005021370016582198</v>
       </c>
       <c r="D13">
-        <v>0.0009167273663890635</v>
+        <v>0.0007045488162801379</v>
       </c>
       <c r="E13">
-        <v>0.0001578654377165457</v>
+        <v>8.758203517294533E-05</v>
       </c>
       <c r="F13">
-        <v>0.000213256819371474</v>
+        <v>0.0002179819542082195</v>
       </c>
       <c r="G13">
-        <v>0.0009305752118027956</v>
+        <v>0.0006500533277280831</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.0001357088850545744</v>
+        <v>0.0001226148492421235</v>
       </c>
       <c r="J13">
-        <v>0.0002021785430404883</v>
+        <v>9.342083751780834E-05</v>
       </c>
       <c r="K13">
-        <v>0.00503784616151573</v>
+        <v>0.002705311753119867</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>0.0002714177701091487</v>
+        <v>0.0003250266638640416</v>
       </c>
       <c r="N13">
-        <v>0.001121675478512298</v>
+        <v>0.0006442145253832201</v>
       </c>
       <c r="O13">
-        <v>0.0002326438029506989</v>
+        <v>0.0001693252680010276</v>
       </c>
       <c r="P13">
-        <v>0.0008004054649137141</v>
+        <v>0.003501335139469525</v>
       </c>
       <c r="Q13">
-        <v>0.01052990165260187</v>
+        <v>0.009618453729437685</v>
       </c>
       <c r="R13">
-        <v>0.0004209745005774551</v>
+        <v>0.0003814684198643841</v>
       </c>
       <c r="S13">
-        <v>0.002478764329058042</v>
+        <v>0.001880094355045893</v>
       </c>
       <c r="T13">
-        <v>0.0008557968465686424</v>
+        <v>0.000901121828557193</v>
       </c>
       <c r="U13">
-        <v>0.001116136340346805</v>
+        <v>0.0008583039446948641</v>
       </c>
       <c r="V13">
-        <v>0.002290433631431285</v>
+        <v>0.001331246934628769</v>
       </c>
       <c r="W13">
-        <v>1.107827633098566E-05</v>
+        <v>1.167760468972604E-05</v>
       </c>
       <c r="X13">
-        <v>4.154353624119623E-05</v>
+        <v>4.47641513106165E-05</v>
       </c>
       <c r="Y13">
-        <v>0.000279726477357388</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="Z13">
-        <v>0.0001107827633098566</v>
+        <v>0.0002374446286910962</v>
       </c>
       <c r="AA13">
-        <v>3.046525991021057E-05</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="AB13">
         <v>0</v>
@@ -1813,16 +1813,16 @@
         <v>0</v>
       </c>
       <c r="AE13">
-        <v>0</v>
+        <v>2.140894193116441E-05</v>
       </c>
       <c r="AF13">
-        <v>6.923922706866039E-05</v>
+        <v>9.73133724143837E-05</v>
       </c>
       <c r="AG13">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AH13">
-        <v>3.877396715844982E-05</v>
+        <v>9.73133724143837E-05</v>
       </c>
     </row>
     <row r="14" spans="1:34">
@@ -1830,103 +1830,103 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.005843790764594937</v>
+        <v>0.006753548045558228</v>
       </c>
       <c r="C14">
-        <v>0.0002991134609366129</v>
+        <v>0.0002997251870363018</v>
       </c>
       <c r="D14">
-        <v>0.0009388839190510349</v>
+        <v>0.0007804532467633572</v>
       </c>
       <c r="E14">
-        <v>0.0003849701025017518</v>
+        <v>0.0004865668620719185</v>
       </c>
       <c r="F14">
-        <v>0.0002991134609366129</v>
+        <v>0.0002763699776568497</v>
       </c>
       <c r="G14">
-        <v>0.005705312310457616</v>
+        <v>0.004863722353270897</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="I14">
-        <v>0.0003074221681848521</v>
+        <v>0.0003775758849678087</v>
       </c>
       <c r="J14">
-        <v>0.0002243350957024596</v>
+        <v>0.0001868416750356167</v>
       </c>
       <c r="K14">
-        <v>0.009771039723929354</v>
+        <v>0.008532436493293162</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0.0009721187480439919</v>
+        <v>0.0009711874566955493</v>
       </c>
       <c r="N14">
-        <v>0.0005151398493908332</v>
+        <v>0.0002841550474500004</v>
       </c>
       <c r="O14">
-        <v>0.0001689437140475313</v>
+        <v>0.0001926804773804797</v>
       </c>
       <c r="P14">
-        <v>0.001102288494933073</v>
+        <v>0.0009867575962818507</v>
       </c>
       <c r="Q14">
-        <v>0.007447371263505111</v>
+        <v>0.006901464371628092</v>
       </c>
       <c r="R14">
-        <v>0.0008308707248239247</v>
+        <v>0.000638375723038357</v>
       </c>
       <c r="S14">
-        <v>0.0001523262995510528</v>
+        <v>0.0001634864656561646</v>
       </c>
       <c r="T14">
-        <v>0.002365211996665439</v>
+        <v>0.002395855228842126</v>
       </c>
       <c r="U14">
-        <v>0.0004071266551637231</v>
+        <v>0.0003425430708986306</v>
       </c>
       <c r="V14">
-        <v>0.001786372058371438</v>
+        <v>0.001718554156838016</v>
       </c>
       <c r="W14">
-        <v>3.877396715844982E-05</v>
+        <v>2.919401172431511E-05</v>
       </c>
       <c r="X14">
-        <v>4.985224348943548E-05</v>
+        <v>3.69790815174658E-05</v>
       </c>
       <c r="Y14">
-        <v>1.938698357922491E-05</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="Z14">
-        <v>0.0004098962242464695</v>
+        <v>0.0007240114907630147</v>
       </c>
       <c r="AA14">
-        <v>6.370008890316756E-05</v>
+        <v>2.724774427602743E-05</v>
       </c>
       <c r="AB14">
-        <v>5.539138165492831E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="AC14">
         <v>0</v>
       </c>
       <c r="AD14">
-        <v>0.0006896227016038575</v>
+        <v>0.000805754723591097</v>
       </c>
       <c r="AE14">
-        <v>0.005328650915204103</v>
+        <v>0.004554265828993157</v>
       </c>
       <c r="AF14">
-        <v>6.923922706866039E-05</v>
+        <v>9.73133724143837E-05</v>
       </c>
       <c r="AG14">
-        <v>0.00113552332392603</v>
+        <v>0.001132727654903426</v>
       </c>
       <c r="AH14">
-        <v>0.002032863706735869</v>
+        <v>0.001819760064148975</v>
       </c>
     </row>
     <row r="15" spans="1:34">
@@ -1934,103 +1934,103 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.004245749403850255</v>
+        <v>0.002841550474500004</v>
       </c>
       <c r="C15">
-        <v>0.0006563878726109005</v>
+        <v>0.0003444893383469183</v>
       </c>
       <c r="D15">
-        <v>0.0008862621064788529</v>
+        <v>0.0008816591540743163</v>
       </c>
       <c r="E15">
-        <v>0.0003628135498397804</v>
+        <v>0.0003133490591743155</v>
       </c>
       <c r="F15">
-        <v>0.0003877396715844981</v>
+        <v>0.0005099220714513705</v>
       </c>
       <c r="G15">
-        <v>0.004522706312124897</v>
+        <v>0.005192641552031514</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0.0001301697468890815</v>
+        <v>0.000173217802897603</v>
       </c>
       <c r="J15">
-        <v>0.0002492612174471774</v>
+        <v>0.0002043580820702058</v>
       </c>
       <c r="K15">
-        <v>0.004514397604876657</v>
+        <v>0.003396236697261991</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0.0006425400271971684</v>
+        <v>0.000441802710761302</v>
       </c>
       <c r="N15">
-        <v>0.0003406569971778091</v>
+        <v>0.0002763699776568497</v>
       </c>
       <c r="O15">
-        <v>0.0005234485566390725</v>
+        <v>0.0002899938497948634</v>
       </c>
       <c r="P15">
-        <v>0.001789141627454184</v>
+        <v>0.00296221905629384</v>
       </c>
       <c r="Q15">
-        <v>0.004201436298526312</v>
+        <v>0.005124522191341446</v>
       </c>
       <c r="R15">
-        <v>0.001287849623477083</v>
+        <v>0.0009945426660750013</v>
       </c>
       <c r="S15">
-        <v>0.000360043980757034</v>
+        <v>0.000346435605795206</v>
       </c>
       <c r="T15">
-        <v>0.001035818836947159</v>
+        <v>0.001177491806214043</v>
       </c>
       <c r="U15">
-        <v>0.000326809151764077</v>
+        <v>0.0005118683388996582</v>
       </c>
       <c r="V15">
-        <v>0.002273816216934807</v>
+        <v>0.003071210033397949</v>
       </c>
       <c r="W15">
-        <v>8.031750339964605E-05</v>
+        <v>3.892534896575348E-05</v>
       </c>
       <c r="X15">
-        <v>7.754793431689964E-05</v>
+        <v>8.9528302621233E-05</v>
       </c>
       <c r="Y15">
-        <v>4.985224348943548E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="Z15">
-        <v>0.0002160263884542204</v>
+        <v>0.0005001907342099322</v>
       </c>
       <c r="AA15">
-        <v>8.585664156513888E-05</v>
+        <v>4.671041875890417E-05</v>
       </c>
       <c r="AB15">
-        <v>8.308707248239246E-06</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="AC15">
         <v>0</v>
       </c>
       <c r="AD15">
-        <v>0.0009831970243749774</v>
+        <v>0.00100427400331644</v>
       </c>
       <c r="AE15">
-        <v>0.0001246306087235887</v>
+        <v>8.368950027636998E-05</v>
       </c>
       <c r="AF15">
-        <v>9.416534881337813E-05</v>
+        <v>7.785069793150696E-05</v>
       </c>
       <c r="AG15">
-        <v>1.938698357922491E-05</v>
+        <v>0</v>
       </c>
       <c r="AH15">
-        <v>0.0005151398493908332</v>
+        <v>0.000615020513658905</v>
       </c>
     </row>
     <row r="16" spans="1:34">
@@ -2038,103 +2038,103 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.01118351995613003</v>
+        <v>0.01183135981814077</v>
       </c>
       <c r="C16">
-        <v>0.0002187959575369668</v>
+        <v>0.000262746105518836</v>
       </c>
       <c r="D16">
-        <v>0.0003766613952535125</v>
+        <v>0.0004165012339335622</v>
       </c>
       <c r="E16">
-        <v>0.0003185004445158378</v>
+        <v>0.0001401312562767125</v>
       </c>
       <c r="F16">
-        <v>0.0009527317644647669</v>
+        <v>0.0005352235482791103</v>
       </c>
       <c r="G16">
-        <v>0.00808991129070228</v>
+        <v>0.01348763341663358</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.000180021990378517</v>
+        <v>3.69790815174658E-05</v>
       </c>
       <c r="J16">
-        <v>0.0001911002667095027</v>
+        <v>0.0001401312562767125</v>
       </c>
       <c r="K16">
-        <v>0.008951247275436416</v>
+        <v>0.008801021401156862</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0.000720087961514068</v>
+        <v>0.0005371698157273979</v>
       </c>
       <c r="N16">
-        <v>3.323482899295698E-05</v>
+        <v>4.671041875890417E-05</v>
       </c>
       <c r="O16">
-        <v>0.0001301697468890815</v>
+        <v>0.0001362387213801372</v>
       </c>
       <c r="P16">
-        <v>0.003664139896473508</v>
+        <v>0.003470194860296922</v>
       </c>
       <c r="Q16">
-        <v>0.01186483395048564</v>
+        <v>0.01260792053000755</v>
       </c>
       <c r="R16">
-        <v>0.000360043980757034</v>
+        <v>0.0004203937688301375</v>
       </c>
       <c r="S16">
-        <v>0.00014678716138556</v>
+        <v>0.0001868416750356167</v>
       </c>
       <c r="T16">
-        <v>0.001570345669917218</v>
+        <v>0.0007551517699356175</v>
       </c>
       <c r="U16">
-        <v>0.001514954288262289</v>
+        <v>0.0006519995951763708</v>
       </c>
       <c r="V16">
-        <v>0.002730795115587966</v>
+        <v>0.002787054985947949</v>
       </c>
       <c r="W16">
-        <v>5.816095073767472E-05</v>
+        <v>0.0001557013958630139</v>
       </c>
       <c r="X16">
-        <v>6.646965798591397E-05</v>
+        <v>3.892534896575348E-05</v>
       </c>
       <c r="Y16">
-        <v>0.000653618303528154</v>
+        <v>0.0001926804773804797</v>
       </c>
       <c r="Z16">
-        <v>0.0003822005334190053</v>
+        <v>0.0004787817922787678</v>
       </c>
       <c r="AA16">
-        <v>5.816095073767472E-05</v>
+        <v>3.114027917260278E-05</v>
       </c>
       <c r="AB16">
-        <v>9.970448697887096E-05</v>
+        <v>0.0001362387213801372</v>
       </c>
       <c r="AC16">
-        <v>5.539138165492831E-06</v>
+        <v>0</v>
       </c>
       <c r="AD16">
-        <v>0.005306494362542132</v>
+        <v>0.002973896660983566</v>
       </c>
       <c r="AE16">
-        <v>0.001102288494933073</v>
+        <v>0.001276751446076714</v>
       </c>
       <c r="AF16">
-        <v>3.877396715844982E-05</v>
+        <v>3.503281406917813E-05</v>
       </c>
       <c r="AG16">
-        <v>9.970448697887096E-05</v>
+        <v>0.0002004655471736304</v>
       </c>
       <c r="AH16">
-        <v>0.001177066860167227</v>
+        <v>0.004015149745817471</v>
       </c>
     </row>
     <row r="17" spans="1:34">
@@ -2142,103 +2142,103 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.0002852656155228808</v>
+        <v>0.000268584907863699</v>
       </c>
       <c r="C17">
-        <v>0.005195711599232275</v>
+        <v>0.00534639668044624</v>
       </c>
       <c r="D17">
-        <v>0.01204485594086416</v>
+        <v>0.01173793898062296</v>
       </c>
       <c r="E17">
-        <v>0.005536368596410084</v>
+        <v>0.006284497590520899</v>
       </c>
       <c r="F17">
-        <v>0.007466758247084336</v>
+        <v>0.006393488567625009</v>
       </c>
       <c r="G17">
-        <v>0.002215655266197132</v>
+        <v>0.0032210726269161</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="I17">
-        <v>0.0022793553551003</v>
+        <v>0.003444893383469183</v>
       </c>
       <c r="J17">
-        <v>0.002207346558948893</v>
+        <v>0.001870363017804455</v>
       </c>
       <c r="K17">
-        <v>0.001805759041950663</v>
+        <v>0.002629407322636647</v>
       </c>
       <c r="L17">
-        <v>0.004511628035793911</v>
+        <v>0.003224965161812675</v>
       </c>
       <c r="M17">
-        <v>0.003536739718667173</v>
+        <v>0.003477979930090073</v>
       </c>
       <c r="N17">
-        <v>0.007616314977552643</v>
+        <v>0.006412951242107886</v>
       </c>
       <c r="O17">
-        <v>0.007308892809367791</v>
+        <v>0.007238168640181859</v>
       </c>
       <c r="P17">
-        <v>0.007128870818989274</v>
+        <v>0.009303158402815081</v>
       </c>
       <c r="Q17">
-        <v>0.001609119637075667</v>
+        <v>0.002321897065807195</v>
       </c>
       <c r="R17">
-        <v>0.003866318439513996</v>
+        <v>0.003861394617402745</v>
       </c>
       <c r="S17">
-        <v>0.008593972863762128</v>
+        <v>0.006235840904313708</v>
       </c>
       <c r="T17">
-        <v>0.00981258326017055</v>
+        <v>0.009532817961713026</v>
       </c>
       <c r="U17">
-        <v>0.006990392364851952</v>
+        <v>0.009127994332469191</v>
       </c>
       <c r="V17">
-        <v>0.0005289876948045653</v>
+        <v>0.001050984422075344</v>
       </c>
       <c r="W17">
-        <v>0.0003406569971778091</v>
+        <v>0.0004690504550373294</v>
       </c>
       <c r="X17">
-        <v>0.0008890316755615994</v>
+        <v>0.0006500533277280831</v>
       </c>
       <c r="Y17">
-        <v>0.0003351178590123163</v>
+        <v>0.0002004655471736304</v>
       </c>
       <c r="Z17">
-        <v>0.002434451223734099</v>
+        <v>0.004205883955749663</v>
       </c>
       <c r="AA17">
-        <v>0.001082901511353848</v>
+        <v>0.001049038154627056</v>
       </c>
       <c r="AB17">
-        <v>0.0002741873391918951</v>
+        <v>0.0002316058263462332</v>
       </c>
       <c r="AC17">
         <v>0</v>
       </c>
       <c r="AD17">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AE17">
         <v>0</v>
       </c>
       <c r="AF17">
-        <v>0.000393278809749991</v>
+        <v>0.0004885131295202062</v>
       </c>
       <c r="AG17">
-        <v>0.0002991134609366129</v>
+        <v>0.0006831398743489736</v>
       </c>
       <c r="AH17">
-        <v>0.0008779533992306137</v>
+        <v>0.001473324458353769</v>
       </c>
     </row>
     <row r="18" spans="1:34">
@@ -2246,103 +2246,103 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.002282124924183046</v>
+        <v>0.001584261702906167</v>
       </c>
       <c r="C18">
-        <v>8.308707248239247E-05</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="D18">
-        <v>0.0001107827633098566</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="E18">
-        <v>3.046525991021057E-05</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>4.154353624119623E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="G18">
-        <v>0.003010521592945354</v>
+        <v>0.002547664089808565</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1.384784541373208E-05</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>2.769569082746415E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="K18">
-        <v>0.00176975464387496</v>
+        <v>0.0008972292936606177</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>0.0001218610396408423</v>
+        <v>7.979696537979462E-05</v>
       </c>
       <c r="N18">
-        <v>0.0009721187480439919</v>
+        <v>0.0005060295365547952</v>
       </c>
       <c r="O18">
-        <v>2.769569082746415E-05</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>0.0002824960464401344</v>
+        <v>0.0001303999190352742</v>
       </c>
       <c r="Q18">
-        <v>0.01067114967582194</v>
+        <v>0.01053514569758118</v>
       </c>
       <c r="R18">
-        <v>0.001138292893008777</v>
+        <v>0.0006052891764174665</v>
       </c>
       <c r="S18">
-        <v>0.00727011884220934</v>
+        <v>0.008228818771360285</v>
       </c>
       <c r="T18">
-        <v>0.0002243350957024596</v>
+        <v>2.919401172431511E-05</v>
       </c>
       <c r="U18">
-        <v>0.00014678716138556</v>
+        <v>0.0001829491401390413</v>
       </c>
       <c r="V18">
-        <v>0.001188145136498212</v>
+        <v>0.0007006562813835626</v>
       </c>
       <c r="W18">
-        <v>5.539138165492831E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="X18">
-        <v>1.107827633098566E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="Y18">
-        <v>1.661741449647849E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="Z18">
-        <v>3.323482899295698E-05</v>
+        <v>2.140894193116441E-05</v>
       </c>
       <c r="AA18">
-        <v>1.384784541373208E-05</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="AB18">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AC18">
         <v>0</v>
       </c>
       <c r="AD18">
-        <v>0.0003655831189225268</v>
+        <v>0.0002588535706222606</v>
       </c>
       <c r="AE18">
-        <v>0.000113552332392603</v>
+        <v>7.395816303493161E-05</v>
       </c>
       <c r="AF18">
-        <v>1.661741449647849E-05</v>
+        <v>0</v>
       </c>
       <c r="AG18">
-        <v>1.938698357922491E-05</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="AH18">
-        <v>0.0003877396715844981</v>
+        <v>0.0005955578391760282</v>
       </c>
     </row>
     <row r="19" spans="1:34">
@@ -2350,103 +2350,103 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.009712878773191679</v>
+        <v>0.008012783084600354</v>
       </c>
       <c r="C19">
-        <v>0.0002187959575369668</v>
+        <v>0.0001771103377941783</v>
       </c>
       <c r="D19">
-        <v>0.0006342313199489292</v>
+        <v>0.0005118683388996582</v>
       </c>
       <c r="E19">
-        <v>0.0006425400271971684</v>
+        <v>0.0001829491401390413</v>
       </c>
       <c r="F19">
-        <v>0.0003988179479154838</v>
+        <v>0.000906960630902056</v>
       </c>
       <c r="G19">
-        <v>0.006990392364851952</v>
+        <v>0.006033429089691789</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0.0004015875169982303</v>
+        <v>0.0003152953266226031</v>
       </c>
       <c r="J19">
-        <v>0.0001911002667095027</v>
+        <v>5.838802344863021E-05</v>
       </c>
       <c r="K19">
-        <v>0.006076434567545636</v>
+        <v>0.00543008618072261</v>
       </c>
       <c r="L19">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>0.0005899182146249866</v>
+        <v>0.0002724774427602743</v>
       </c>
       <c r="N19">
-        <v>0.0001634045758820385</v>
+        <v>7.006562813835626E-05</v>
       </c>
       <c r="O19">
-        <v>0.0007007009779348431</v>
+        <v>0.0002510685008291099</v>
       </c>
       <c r="P19">
-        <v>0.001847302578191859</v>
+        <v>0.0007687756420736312</v>
       </c>
       <c r="Q19">
-        <v>0.009953831283390618</v>
+        <v>0.00827552919011919</v>
       </c>
       <c r="R19">
-        <v>0.0003295787208468234</v>
+        <v>0.0002257670240013702</v>
       </c>
       <c r="S19">
-        <v>0.0001938698357922491</v>
+        <v>9.147457006952067E-05</v>
       </c>
       <c r="T19">
-        <v>0.0009527317644647669</v>
+        <v>0.0001946267448287674</v>
       </c>
       <c r="U19">
-        <v>0.0009250360736373028</v>
+        <v>0.0005157608737962336</v>
       </c>
       <c r="V19">
-        <v>0.003187774014241124</v>
+        <v>0.00276953857891336</v>
       </c>
       <c r="W19">
-        <v>7.20087961514068E-05</v>
+        <v>8.368950027636998E-05</v>
       </c>
       <c r="X19">
-        <v>0.0002548003556126702</v>
+        <v>6.811936069006858E-05</v>
       </c>
       <c r="Y19">
-        <v>6.646965798591397E-05</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="Z19">
-        <v>0.0001163219014753494</v>
+        <v>9.147457006952067E-05</v>
       </c>
       <c r="AA19">
-        <v>0.0002852656155228808</v>
+        <v>0.0003444893383469183</v>
       </c>
       <c r="AB19">
-        <v>4.431310532394265E-05</v>
+        <v>1.751640703458906E-05</v>
       </c>
       <c r="AC19">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AD19">
-        <v>0.001728211107633763</v>
+        <v>0.001056823224420207</v>
       </c>
       <c r="AE19">
-        <v>0.0005871486455422401</v>
+        <v>0.001117157515317125</v>
       </c>
       <c r="AF19">
-        <v>1.661741449647849E-05</v>
+        <v>7.785069793150696E-06</v>
       </c>
       <c r="AG19">
-        <v>0.0001772524212957706</v>
+        <v>0.0002510685008291099</v>
       </c>
       <c r="AH19">
-        <v>0.001038588406029906</v>
+        <v>0.001148297794489728</v>
       </c>
     </row>
     <row r="20" spans="1:34">
@@ -2454,103 +2454,103 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.002185190006286922</v>
+        <v>0.002222637425944524</v>
       </c>
       <c r="C20">
-        <v>0.0002437220792816846</v>
+        <v>0.0001829491401390413</v>
       </c>
       <c r="D20">
-        <v>0.001681128433227074</v>
+        <v>0.001811974994355824</v>
       </c>
       <c r="E20">
-        <v>0.0001966394048749955</v>
+        <v>0.0001595939307595892</v>
       </c>
       <c r="F20">
-        <v>0.0003295787208468234</v>
+        <v>0.0003853609547609594</v>
       </c>
       <c r="G20">
-        <v>0.003196082721489363</v>
+        <v>0.004647686666510965</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>0.00081159352593596</v>
       </c>
       <c r="I20">
-        <v>0.0001107827633098566</v>
+        <v>0.0002705311753119867</v>
       </c>
       <c r="J20">
-        <v>0.0001052436251443638</v>
+        <v>7.590443048321929E-05</v>
       </c>
       <c r="K20">
-        <v>0.002390138118410157</v>
+        <v>0.001671843738079112</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>0.006325695784992813</v>
+        <v>0.004100785513542129</v>
       </c>
       <c r="N20">
-        <v>0.002567390539705927</v>
+        <v>0.003622003721263361</v>
       </c>
       <c r="O20">
-        <v>0.0008807229683133602</v>
+        <v>0.00150641100497466</v>
       </c>
       <c r="P20">
-        <v>0.001459562906607361</v>
+        <v>0.001677682540423975</v>
       </c>
       <c r="Q20">
-        <v>0.003835853179603786</v>
+        <v>0.003149060731329456</v>
       </c>
       <c r="R20">
-        <v>0.002462146914561563</v>
+        <v>0.002380285089255825</v>
       </c>
       <c r="S20">
-        <v>0.0004985224348943547</v>
+        <v>0.0002471759659325346</v>
       </c>
       <c r="T20">
-        <v>0.001833454732778127</v>
+        <v>0.001169706736420892</v>
       </c>
       <c r="U20">
-        <v>0.01411649361475848</v>
+        <v>0.01185082249262365</v>
       </c>
       <c r="V20">
-        <v>0.0009804274552922311</v>
+        <v>0.0008660890144880149</v>
       </c>
       <c r="W20">
-        <v>6.093051982042114E-05</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="X20">
-        <v>0.0002354133720334453</v>
+        <v>0.0002354983612428085</v>
       </c>
       <c r="Y20">
-        <v>0.0001218610396408423</v>
+        <v>5.449548855205487E-05</v>
       </c>
       <c r="Z20">
-        <v>0.0004126657933292159</v>
+        <v>0.000632536920693494</v>
       </c>
       <c r="AA20">
-        <v>0.0001190914705580959</v>
+        <v>0.0001459700586215755</v>
       </c>
       <c r="AB20">
         <v>0</v>
       </c>
       <c r="AC20">
-        <v>4.154353624119623E-05</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="AD20">
-        <v>0.0005096007112253405</v>
+        <v>0.0002121431518633564</v>
       </c>
       <c r="AE20">
-        <v>0.003187774014241124</v>
+        <v>0.003884749826782197</v>
       </c>
       <c r="AF20">
-        <v>5.816095073767472E-05</v>
+        <v>6.228055834520557E-05</v>
       </c>
       <c r="AG20">
-        <v>0.0002548003556126702</v>
+        <v>0.000262746105518836</v>
       </c>
       <c r="AH20">
-        <v>0.003954944650161881</v>
+        <v>0.004460844991475348</v>
       </c>
     </row>
     <row r="21" spans="1:34">
@@ -2558,103 +2558,103 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.007846189211420595</v>
+        <v>0.007146694070112339</v>
       </c>
       <c r="C21">
-        <v>0.0002935743227711201</v>
+        <v>0.0005780414321414391</v>
       </c>
       <c r="D21">
-        <v>0.003996488186403077</v>
+        <v>0.003353418813399662</v>
       </c>
       <c r="E21">
-        <v>0.0001301697468890815</v>
+        <v>0.0001303999190352742</v>
       </c>
       <c r="F21">
-        <v>0.0004652876059013978</v>
+        <v>0.0003873072222092471</v>
       </c>
       <c r="G21">
-        <v>0.006915613999617799</v>
+        <v>0.006965691197421585</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>7.754793431689964E-05</v>
+        <v>9.73133724143837E-05</v>
       </c>
       <c r="J21">
-        <v>0.0001384784541373208</v>
+        <v>0.0001693252680010276</v>
       </c>
       <c r="K21">
-        <v>0.004810741496730523</v>
+        <v>0.004933787981409254</v>
       </c>
       <c r="L21">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="M21">
-        <v>0.0009416534881337813</v>
+        <v>0.0007493129675907544</v>
       </c>
       <c r="N21">
-        <v>0.0003129613063503449</v>
+        <v>0.0004028773617955485</v>
       </c>
       <c r="O21">
-        <v>0.0008779533992306137</v>
+        <v>0.0002510685008291099</v>
       </c>
       <c r="P21">
-        <v>0.002138107331880233</v>
+        <v>0.001702984017251715</v>
       </c>
       <c r="Q21">
-        <v>0.01123060263053671</v>
+        <v>0.01787257397762571</v>
       </c>
       <c r="R21">
-        <v>0.0006951618397693503</v>
+        <v>0.0006305906532452063</v>
       </c>
       <c r="S21">
-        <v>0.004290062509174197</v>
+        <v>0.002993359335466443</v>
       </c>
       <c r="T21">
-        <v>0.001808528611033409</v>
+        <v>0.001948213715735962</v>
       </c>
       <c r="U21">
-        <v>0.0003046525991021057</v>
+        <v>0.0004651579201407541</v>
       </c>
       <c r="V21">
-        <v>0.00250369045080276</v>
+        <v>0.001847007808425003</v>
       </c>
       <c r="W21">
-        <v>4.431310532394265E-05</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="X21">
-        <v>4.708267440668906E-05</v>
+        <v>4.281788386232883E-05</v>
       </c>
       <c r="Y21">
-        <v>0.000113552332392603</v>
+        <v>5.254922110376719E-05</v>
       </c>
       <c r="Z21">
-        <v>0.0002824960464401344</v>
+        <v>0.0006461607928315077</v>
       </c>
       <c r="AA21">
-        <v>4.985224348943548E-05</v>
+        <v>2.724774427602743E-05</v>
       </c>
       <c r="AB21">
-        <v>1.661741449647849E-05</v>
+        <v>3.308654662089046E-05</v>
       </c>
       <c r="AC21">
-        <v>1.384784541373208E-05</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="AD21">
-        <v>0.001775293782040452</v>
+        <v>0.001414936434905139</v>
       </c>
       <c r="AE21">
-        <v>0.004641797782682993</v>
+        <v>0.007818156339771586</v>
       </c>
       <c r="AF21">
-        <v>8.031750339964605E-05</v>
+        <v>0.0001887879424839044</v>
       </c>
       <c r="AG21">
-        <v>0.0001717132831302778</v>
+        <v>5.838802344863021E-05</v>
       </c>
       <c r="AH21">
-        <v>0.000573300800128508</v>
+        <v>0.0007045488162801379</v>
       </c>
     </row>
     <row r="22" spans="1:34">
@@ -2662,85 +2662,85 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.0002631090628609095</v>
+        <v>0.0002199282216565072</v>
       </c>
       <c r="C22">
-        <v>0.001498336873765811</v>
+        <v>0.0007590443048321929</v>
       </c>
       <c r="D22">
-        <v>0.001179836429249973</v>
+        <v>0.001558960226078427</v>
       </c>
       <c r="E22">
-        <v>0.0009831970243749774</v>
+        <v>0.001813921261804112</v>
       </c>
       <c r="F22">
-        <v>0.002168572591790443</v>
+        <v>0.002282971716841442</v>
       </c>
       <c r="G22">
-        <v>0.0004403614841566801</v>
+        <v>0.0003561669430366443</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0.001606350067992921</v>
+        <v>0.002024118146219181</v>
       </c>
       <c r="J22">
-        <v>0.0007283966687623072</v>
+        <v>0.0005021370016582198</v>
       </c>
       <c r="K22">
-        <v>0.0006425400271971684</v>
+        <v>0.0006052891764174665</v>
       </c>
       <c r="L22">
-        <v>0.0001274001778063351</v>
+        <v>0.0001829491401390413</v>
       </c>
       <c r="M22">
-        <v>0.00157588480808271</v>
+        <v>0.001109372445523974</v>
       </c>
       <c r="N22">
-        <v>0.002298742338679525</v>
+        <v>0.001360440946353084</v>
       </c>
       <c r="O22">
-        <v>0.001370936695959476</v>
+        <v>0.001915127169115071</v>
       </c>
       <c r="P22">
-        <v>0.001179836429249973</v>
+        <v>0.001150244061938015</v>
       </c>
       <c r="Q22">
-        <v>0.0004292832078256944</v>
+        <v>0.0004184475013818499</v>
       </c>
       <c r="R22">
-        <v>0.001681128433227074</v>
+        <v>0.001268966376283563</v>
       </c>
       <c r="S22">
-        <v>0.001465102044772854</v>
+        <v>0.0006714622696592475</v>
       </c>
       <c r="T22">
-        <v>0.002082715950225304</v>
+        <v>0.001578422900561304</v>
       </c>
       <c r="U22">
-        <v>0.001836224301860874</v>
+        <v>0.002251831437668839</v>
       </c>
       <c r="V22">
-        <v>0.0001578654377165457</v>
+        <v>0.0001771103377941783</v>
       </c>
       <c r="W22">
-        <v>8.308707248239247E-05</v>
+        <v>3.308654662089046E-05</v>
       </c>
       <c r="X22">
-        <v>0.0006619270107763933</v>
+        <v>0.0004184475013818499</v>
       </c>
       <c r="Y22">
-        <v>3.60043980757034E-05</v>
+        <v>1.167760468972604E-05</v>
       </c>
       <c r="Z22">
-        <v>0.001210301689160184</v>
+        <v>0.001414936434905139</v>
       </c>
       <c r="AA22">
-        <v>0.0007920967576654748</v>
+        <v>0.0006500533277280831</v>
       </c>
       <c r="AB22">
-        <v>0.0003074221681848521</v>
+        <v>0.0002977789195880141</v>
       </c>
       <c r="AC22">
         <v>0</v>
@@ -2752,13 +2752,13 @@
         <v>0</v>
       </c>
       <c r="AF22">
-        <v>7.477836523415322E-05</v>
+        <v>9.925963986267137E-05</v>
       </c>
       <c r="AG22">
-        <v>0.001262923501732366</v>
+        <v>0.0009264233053849327</v>
       </c>
       <c r="AH22">
-        <v>0.0001634045758820385</v>
+        <v>0.0001595939307595892</v>
       </c>
     </row>
     <row r="23" spans="1:34">
@@ -2766,22 +2766,22 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.0003406569971778091</v>
+        <v>0.0002218744891047948</v>
       </c>
       <c r="C23">
-        <v>2.769569082746416E-06</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="D23">
-        <v>5.539138165492831E-06</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="E23">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>2.769569082746416E-06</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="G23">
-        <v>0.000526218125721819</v>
+        <v>0.0003814684198643841</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2790,46 +2790,46 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>8.308707248239246E-06</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="K23">
-        <v>0.0005096007112253405</v>
+        <v>0.0004982444667616445</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="N23">
-        <v>8.308707248239247E-05</v>
+        <v>1.167760468972604E-05</v>
       </c>
       <c r="O23">
-        <v>5.539138165492831E-06</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="P23">
-        <v>1.938698357922491E-05</v>
+        <v>2.140894193116441E-05</v>
       </c>
       <c r="Q23">
-        <v>0.0004819050203978763</v>
+        <v>0.0001031521747592467</v>
       </c>
       <c r="R23">
-        <v>1.661741449647849E-05</v>
+        <v>0</v>
       </c>
       <c r="S23">
-        <v>0.0002437220792816846</v>
+        <v>9.342083751780834E-05</v>
       </c>
       <c r="T23">
-        <v>6.093051982042114E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="U23">
-        <v>2.769569082746415E-05</v>
+        <v>2.335520937945209E-05</v>
       </c>
       <c r="V23">
-        <v>9.693491789612454E-05</v>
+        <v>6.422682579349324E-05</v>
       </c>
       <c r="W23">
-        <v>1.938698357922491E-05</v>
+        <v>2.140894193116441E-05</v>
       </c>
       <c r="X23">
         <v>0</v>
@@ -2850,19 +2850,19 @@
         <v>0</v>
       </c>
       <c r="AD23">
-        <v>1.938698357922491E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="AE23">
-        <v>1.938698357922491E-05</v>
+        <v>0.0002880475823465757</v>
       </c>
       <c r="AF23">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AG23">
-        <v>8.308707248239246E-06</v>
+        <v>0</v>
       </c>
       <c r="AH23">
-        <v>0</v>
+        <v>1.946267448287674E-06</v>
       </c>
     </row>
     <row r="24" spans="1:34">
@@ -2870,88 +2870,88 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.0009111882282235707</v>
+        <v>0.0005760951646931515</v>
       </c>
       <c r="C24">
-        <v>0.0001744828522130242</v>
+        <v>0.0001031521747592467</v>
       </c>
       <c r="D24">
-        <v>0.0005622225237975223</v>
+        <v>0.0005235459435893843</v>
       </c>
       <c r="E24">
-        <v>0.0001634045758820385</v>
+        <v>0.000101205907310959</v>
       </c>
       <c r="F24">
-        <v>0.0001827915594612634</v>
+        <v>0.0002063043495184934</v>
       </c>
       <c r="G24">
-        <v>0.0001301697468890815</v>
+        <v>0.0001381849888284248</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>5.816095073767472E-05</v>
+        <v>3.503281406917813E-05</v>
       </c>
       <c r="J24">
-        <v>8.308707248239247E-05</v>
+        <v>7.590443048321929E-05</v>
       </c>
       <c r="K24">
-        <v>0.0006785444252728718</v>
+        <v>0.0003970385594506855</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
-        <v>0.0002658786319436559</v>
+        <v>0.0001985192797253427</v>
       </c>
       <c r="N24">
-        <v>0.0002963438918538664</v>
+        <v>0.0001810028726907537</v>
       </c>
       <c r="O24">
-        <v>0.0003655831189225268</v>
+        <v>0.0002004655471736304</v>
       </c>
       <c r="P24">
-        <v>0.000459748467735905</v>
+        <v>0.0004126086990369868</v>
       </c>
       <c r="Q24">
-        <v>0.00278895606632564</v>
+        <v>0.002892153428155483</v>
       </c>
       <c r="R24">
-        <v>0.0005372964020528046</v>
+        <v>0.0003328117336571923</v>
       </c>
       <c r="S24">
-        <v>0.0003378874280950627</v>
+        <v>0.0001537551284147262</v>
       </c>
       <c r="T24">
-        <v>0.0005151398493908332</v>
+        <v>0.0003775758849678087</v>
       </c>
       <c r="U24">
-        <v>0.0002548003556126702</v>
+        <v>0.0001440237911732879</v>
       </c>
       <c r="V24">
-        <v>0.0003711222570880197</v>
+        <v>0.0001985192797253427</v>
       </c>
       <c r="W24">
-        <v>3.323482899295698E-05</v>
+        <v>2.335520937945209E-05</v>
       </c>
       <c r="X24">
-        <v>1.384784541373208E-05</v>
+        <v>2.530147682773976E-05</v>
       </c>
       <c r="Y24">
-        <v>2.492612174471774E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="Z24">
-        <v>5.816095073767472E-05</v>
+        <v>7.590443048321929E-05</v>
       </c>
       <c r="AA24">
-        <v>8.031750339964605E-05</v>
+        <v>2.530147682773976E-05</v>
       </c>
       <c r="AB24">
-        <v>2.769569082746416E-06</v>
+        <v>7.785069793150696E-06</v>
       </c>
       <c r="AC24">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AD24">
         <v>0</v>
@@ -2960,13 +2960,13 @@
         <v>0</v>
       </c>
       <c r="AF24">
-        <v>7.477836523415322E-05</v>
+        <v>4.087161641404115E-05</v>
       </c>
       <c r="AG24">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AH24">
-        <v>1.661741449647849E-05</v>
+        <v>5.060295365547952E-05</v>
       </c>
     </row>
     <row r="25" spans="1:34">
@@ -2974,103 +2974,103 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.001010892715202442</v>
+        <v>0.0006597846649695215</v>
       </c>
       <c r="C25">
-        <v>2.215655266197132E-05</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="D25">
-        <v>0.0002243350957024596</v>
+        <v>8.368950027636998E-05</v>
       </c>
       <c r="E25">
-        <v>1.107827633098566E-05</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="F25">
-        <v>2.492612174471774E-05</v>
+        <v>1.167760468972604E-05</v>
       </c>
       <c r="G25">
-        <v>0.001226919103656662</v>
+        <v>0.0007823995142116449</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <v>2.769569082746416E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="J25">
-        <v>1.661741449647849E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="K25">
-        <v>0.001478949890186586</v>
+        <v>0.0002024118146219181</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>0.0003711222570880197</v>
+        <v>0.0001089909771041097</v>
       </c>
       <c r="N25">
-        <v>8.308707248239246E-06</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="O25">
-        <v>2.215655266197132E-05</v>
+        <v>1.167760468972604E-05</v>
       </c>
       <c r="P25">
-        <v>1.938698357922491E-05</v>
+        <v>4.087161641404115E-05</v>
       </c>
       <c r="Q25">
-        <v>0.0002354133720334453</v>
+        <v>0.0002977789195880141</v>
       </c>
       <c r="R25">
-        <v>4.154353624119623E-05</v>
+        <v>4.865668620719185E-05</v>
       </c>
       <c r="S25">
-        <v>1.384784541373208E-05</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="T25">
-        <v>4.708267440668906E-05</v>
+        <v>4.47641513106165E-05</v>
       </c>
       <c r="U25">
-        <v>1.661741449647849E-05</v>
+        <v>1.751640703458906E-05</v>
       </c>
       <c r="V25">
-        <v>0.0003129613063503449</v>
+        <v>0.0001829491401390413</v>
       </c>
       <c r="W25">
-        <v>0.0001550958686337993</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="X25">
-        <v>5.539138165492831E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="Y25">
-        <v>8.308707248239246E-06</v>
+        <v>0</v>
       </c>
       <c r="Z25">
-        <v>5.539138165492831E-06</v>
+        <v>1.751640703458906E-05</v>
       </c>
       <c r="AA25">
-        <v>0</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="AB25">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AC25">
         <v>0</v>
       </c>
       <c r="AD25">
-        <v>0.0003018830300193593</v>
+        <v>0.0002374446286910962</v>
       </c>
       <c r="AE25">
         <v>0</v>
       </c>
       <c r="AF25">
-        <v>2.769569082746416E-06</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="AG25">
         <v>0</v>
       </c>
       <c r="AH25">
-        <v>0</v>
+        <v>7.785069793150696E-06</v>
       </c>
     </row>
     <row r="26" spans="1:34">
@@ -3078,85 +3078,85 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.002639399335857334</v>
+        <v>0.003417645639193155</v>
       </c>
       <c r="C26">
-        <v>3.877396715844982E-05</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="D26">
-        <v>0.0001080131942271102</v>
+        <v>7.201189558664393E-05</v>
       </c>
       <c r="E26">
-        <v>1.938698357922491E-05</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="F26">
-        <v>3.60043980757034E-05</v>
+        <v>4.281788386232883E-05</v>
       </c>
       <c r="G26">
-        <v>0.003819235765107307</v>
+        <v>0.004686612015476719</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
-        <v>8.308707248239246E-06</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>4.708267440668906E-05</v>
+        <v>1.751640703458906E-05</v>
       </c>
       <c r="K26">
-        <v>0.002007937584991151</v>
+        <v>0.002029956948564044</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26">
-        <v>0.0007477836523415322</v>
+        <v>0.0003191878615191785</v>
       </c>
       <c r="N26">
-        <v>0.0001080131942271102</v>
+        <v>4.865668620719185E-05</v>
       </c>
       <c r="O26">
-        <v>3.323482899295698E-05</v>
+        <v>1.946267448287674E-05</v>
       </c>
       <c r="P26">
-        <v>0.001190914705580959</v>
+        <v>0.001017897875454454</v>
       </c>
       <c r="Q26">
-        <v>0.0001717132831302778</v>
+        <v>0.0001245611166904111</v>
       </c>
       <c r="R26">
-        <v>0.00014678716138556</v>
+        <v>6.811936069006858E-05</v>
       </c>
       <c r="S26">
-        <v>0.0001440175923028136</v>
+        <v>0.0004184475013818499</v>
       </c>
       <c r="T26">
-        <v>0.0001274001778063351</v>
+        <v>6.228055834520557E-05</v>
       </c>
       <c r="U26">
-        <v>0.001996859308660166</v>
+        <v>0.005533238355481857</v>
       </c>
       <c r="V26">
-        <v>0.0005456051093010438</v>
+        <v>0.0007785069793150696</v>
       </c>
       <c r="W26">
-        <v>1.107827633098566E-05</v>
+        <v>0</v>
       </c>
       <c r="X26">
-        <v>0</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="Y26">
         <v>0</v>
       </c>
       <c r="Z26">
-        <v>4.154353624119623E-05</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="AA26">
-        <v>8.308707248239247E-05</v>
+        <v>0.0001810028726907537</v>
       </c>
       <c r="AB26">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AC26">
         <v>0</v>
@@ -3165,16 +3165,16 @@
         <v>0</v>
       </c>
       <c r="AE26">
-        <v>0.0003101917372675986</v>
+        <v>0.0002296595588979455</v>
       </c>
       <c r="AF26">
-        <v>5.539138165492831E-06</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="AG26">
         <v>0</v>
       </c>
       <c r="AH26">
-        <v>1.107827633098566E-05</v>
+        <v>5.838802344863021E-06</v>
       </c>
     </row>
     <row r="27" spans="1:34">
@@ -3182,79 +3182,79 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.00128231048531159</v>
+        <v>0.000990650131178426</v>
       </c>
       <c r="C27">
-        <v>1.384784541373208E-05</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="D27">
-        <v>5.262181257218189E-05</v>
+        <v>7.395816303493161E-05</v>
       </c>
       <c r="E27">
-        <v>1.107827633098566E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="F27">
-        <v>5.539138165492831E-06</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>0.002340285874920721</v>
+        <v>0.002514577543187675</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="J27">
         <v>0</v>
       </c>
       <c r="K27">
-        <v>0.001844533009109113</v>
+        <v>0.001782780982631509</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <v>0.0005179094184735797</v>
+        <v>0.0005936115717277405</v>
       </c>
       <c r="N27">
-        <v>0.0005843790764594937</v>
+        <v>0.0006033429089691789</v>
       </c>
       <c r="O27">
-        <v>1.661741449647849E-05</v>
+        <v>2.140894193116441E-05</v>
       </c>
       <c r="P27">
-        <v>0.0004542093295704122</v>
+        <v>0.0004223400362784252</v>
       </c>
       <c r="Q27">
-        <v>0.0003655831189225268</v>
+        <v>0.0002861013148982881</v>
       </c>
       <c r="R27">
-        <v>5.262181257218189E-05</v>
+        <v>2.724774427602743E-05</v>
       </c>
       <c r="S27">
-        <v>5.539138165492831E-06</v>
+        <v>1.167760468972604E-05</v>
       </c>
       <c r="T27">
-        <v>8.308707248239246E-06</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="U27">
-        <v>0.0001634045758820385</v>
+        <v>4.087161641404115E-05</v>
       </c>
       <c r="V27">
-        <v>0.0004237440696602016</v>
+        <v>0.0003230803964157539</v>
       </c>
       <c r="W27">
-        <v>2.769569082746416E-06</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="X27">
-        <v>8.308707248239246E-06</v>
+        <v>0</v>
       </c>
       <c r="Y27">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="Z27">
-        <v>8.308707248239246E-06</v>
+        <v>0</v>
       </c>
       <c r="AA27">
         <v>0</v>
@@ -3269,16 +3269,16 @@
         <v>0</v>
       </c>
       <c r="AE27">
-        <v>0.0002326438029506989</v>
+        <v>0.0005235459435893843</v>
       </c>
       <c r="AF27">
         <v>0</v>
       </c>
       <c r="AG27">
-        <v>1.107827633098566E-05</v>
+        <v>0</v>
       </c>
       <c r="AH27">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:34">
@@ -3286,85 +3286,85 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.0005123702803080869</v>
+        <v>0.0003405968034503429</v>
       </c>
       <c r="C28">
-        <v>2.492612174471774E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="D28">
-        <v>1.938698357922491E-05</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>1.107827633098566E-05</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>7.785069793150696E-06</v>
       </c>
       <c r="G28">
-        <v>0.001393093248621447</v>
+        <v>0.001702984017251715</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <v>0.000933344780885542</v>
+        <v>0.0005527399553136994</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="N28">
         <v>0</v>
       </c>
       <c r="O28">
-        <v>5.539138165492831E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="P28">
-        <v>6.646965798591397E-05</v>
+        <v>6.617309324178092E-05</v>
       </c>
       <c r="Q28">
-        <v>5.539138165492831E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="R28">
-        <v>0</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="S28">
-        <v>8.308707248239246E-06</v>
+        <v>7.785069793150696E-06</v>
       </c>
       <c r="T28">
-        <v>8.308707248239246E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="U28">
-        <v>8.308707248239246E-06</v>
+        <v>0</v>
       </c>
       <c r="V28">
-        <v>0.0001107827633098566</v>
+        <v>0.0001401312562767125</v>
       </c>
       <c r="W28">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="X28">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="Y28">
         <v>0</v>
       </c>
       <c r="Z28">
-        <v>0</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="AA28">
         <v>0</v>
       </c>
       <c r="AB28">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="AC28">
         <v>0</v>
@@ -3373,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="AE28">
-        <v>3.046525991021057E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="AF28">
         <v>0</v>
@@ -3382,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="AH28">
-        <v>0</v>
+        <v>3.892534896575348E-06</v>
       </c>
     </row>
     <row r="29" spans="1:34">
@@ -3393,7 +3393,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -3405,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>0.00014678716138556</v>
+        <v>5.644175600034255E-05</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -3432,19 +3432,19 @@
         <v>0</v>
       </c>
       <c r="P29">
-        <v>5.539138165492831E-06</v>
+        <v>0</v>
       </c>
       <c r="Q29">
         <v>0</v>
       </c>
       <c r="R29">
-        <v>5.539138165492831E-06</v>
+        <v>0</v>
       </c>
       <c r="S29">
         <v>0</v>
       </c>
       <c r="T29">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="U29">
         <v>0</v>
@@ -3483,10 +3483,10 @@
         <v>0</v>
       </c>
       <c r="AG29">
-        <v>1.661741449647849E-05</v>
+        <v>1.946267448287674E-06</v>
       </c>
       <c r="AH29">
-        <v>0.0001246306087235887</v>
+        <v>0.0002491222333808223</v>
       </c>
     </row>
     <row r="30" spans="1:34">
@@ -3494,85 +3494,85 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>9.139577973063171E-05</v>
+        <v>0.0001167760468972604</v>
       </c>
       <c r="C30">
-        <v>0.0004015875169982303</v>
+        <v>0.0003172415940708908</v>
       </c>
       <c r="D30">
-        <v>0.001625737051572146</v>
+        <v>0.001471378190905481</v>
       </c>
       <c r="E30">
-        <v>0.0002852656155228808</v>
+        <v>0.0001946267448287674</v>
       </c>
       <c r="F30">
-        <v>0.0004154353624119623</v>
+        <v>0.0004768355248304801</v>
       </c>
       <c r="G30">
-        <v>0.00173098067671651</v>
+        <v>0.0008077009910393846</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
-        <v>8.308707248239247E-05</v>
+        <v>6.422682579349324E-05</v>
       </c>
       <c r="J30">
-        <v>0.0002437220792816846</v>
+        <v>0.0002393908961393839</v>
       </c>
       <c r="K30">
-        <v>0.0005816095073767472</v>
+        <v>0.0003873072222092471</v>
       </c>
       <c r="L30">
-        <v>0.002379059842079171</v>
+        <v>0.001523927412009249</v>
       </c>
       <c r="M30">
-        <v>0.0004846745894806227</v>
+        <v>0.0005585787576585624</v>
       </c>
       <c r="N30">
-        <v>0.002196268282617907</v>
+        <v>0.002281025449393154</v>
       </c>
       <c r="O30">
-        <v>0.001872228699936577</v>
+        <v>0.001451915516422605</v>
       </c>
       <c r="P30">
-        <v>0.0007782489122517427</v>
+        <v>0.0009536710496609603</v>
       </c>
       <c r="Q30">
-        <v>0.000279726477357388</v>
+        <v>0.0002899938497948634</v>
       </c>
       <c r="R30">
-        <v>0.000900109951892585</v>
+        <v>0.0005079758040030829</v>
       </c>
       <c r="S30">
-        <v>0.0003794309643362589</v>
+        <v>0.0002997251870363018</v>
       </c>
       <c r="T30">
-        <v>0.001246306087235887</v>
+        <v>0.001342924539318495</v>
       </c>
       <c r="U30">
-        <v>0.0008170228794101926</v>
+        <v>0.001389634958077399</v>
       </c>
       <c r="V30">
-        <v>0.0001357088850545744</v>
+        <v>0.0001518088609664386</v>
       </c>
       <c r="W30">
-        <v>2.769569082746415E-05</v>
+        <v>0</v>
       </c>
       <c r="X30">
-        <v>0.001539880410007007</v>
+        <v>0.0009322621077297958</v>
       </c>
       <c r="Y30">
-        <v>1.661741449647849E-05</v>
+        <v>4.47641513106165E-05</v>
       </c>
       <c r="Z30">
-        <v>0.0002769569082746416</v>
+        <v>0.0005215996761410966</v>
       </c>
       <c r="AA30">
-        <v>0.0004902137276461155</v>
+        <v>0.0005585787576585624</v>
       </c>
       <c r="AB30">
-        <v>1.938698357922491E-05</v>
+        <v>0.0001362387213801372</v>
       </c>
       <c r="AC30">
         <v>0</v>
@@ -3584,13 +3584,13 @@
         <v>0</v>
       </c>
       <c r="AF30">
-        <v>5.262181257218189E-05</v>
+        <v>7.785069793150696E-05</v>
       </c>
       <c r="AG30">
         <v>0</v>
       </c>
       <c r="AH30">
-        <v>4.154353624119623E-05</v>
+        <v>6.811936069006858E-05</v>
       </c>
     </row>
     <row r="31" spans="1:34">
@@ -3598,85 +3598,85 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.0001412480232200672</v>
+        <v>0.0002938863846914387</v>
       </c>
       <c r="C31">
-        <v>0.0004292832078256944</v>
+        <v>0.0005118683388996582</v>
       </c>
       <c r="D31">
-        <v>0.001071823235022863</v>
+        <v>0.001586207970354454</v>
       </c>
       <c r="E31">
-        <v>0.0003849701025017518</v>
+        <v>0.0003503281406917813</v>
       </c>
       <c r="F31">
-        <v>0.0005345268329700582</v>
+        <v>0.0006850861417972612</v>
       </c>
       <c r="G31">
-        <v>0.0008613359847341352</v>
+        <v>0.001235879829662673</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31">
-        <v>8.585664156513888E-05</v>
+        <v>8.758203517294533E-05</v>
       </c>
       <c r="J31">
-        <v>0.0004569788986531585</v>
+        <v>0.0004612653852441787</v>
       </c>
       <c r="K31">
-        <v>0.0007948663267482212</v>
+        <v>0.001412990167456851</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31">
-        <v>0.001395862817704193</v>
+        <v>0.002191497146771921</v>
       </c>
       <c r="N31">
-        <v>0.0001190914705580959</v>
+        <v>0.0003055639893811648</v>
       </c>
       <c r="O31">
-        <v>0.0006203834745351971</v>
+        <v>0.0009400471775229465</v>
       </c>
       <c r="P31">
-        <v>0.002614473214112616</v>
+        <v>0.003114027917260278</v>
       </c>
       <c r="Q31">
-        <v>0.0005622225237975223</v>
+        <v>0.0009147457006952067</v>
       </c>
       <c r="R31">
-        <v>0.0009416534881337813</v>
+        <v>0.001272858911180139</v>
       </c>
       <c r="S31">
-        <v>0.0002769569082746416</v>
+        <v>0.0002880475823465757</v>
       </c>
       <c r="T31">
-        <v>0.001611889206158414</v>
+        <v>0.002282971716841442</v>
       </c>
       <c r="U31">
-        <v>0.0005926877837077329</v>
+        <v>0.000961456119454111</v>
       </c>
       <c r="V31">
-        <v>0.0001994089739577419</v>
+        <v>0.0003775758849678087</v>
       </c>
       <c r="W31">
-        <v>8.031750339964605E-05</v>
+        <v>3.503281406917813E-05</v>
       </c>
       <c r="X31">
-        <v>0.0001107827633098566</v>
+        <v>0.000184895407587329</v>
       </c>
       <c r="Y31">
-        <v>0.0001440175923028136</v>
+        <v>9.536710496609602E-05</v>
       </c>
       <c r="Z31">
-        <v>0.0003738918261707661</v>
+        <v>0.0007960233863496586</v>
       </c>
       <c r="AA31">
-        <v>0.0006037660600387186</v>
+        <v>0.0005215996761410966</v>
       </c>
       <c r="AB31">
-        <v>4.985224348943548E-05</v>
+        <v>6.811936069006858E-05</v>
       </c>
       <c r="AC31">
         <v>0</v>
@@ -3688,13 +3688,13 @@
         <v>0</v>
       </c>
       <c r="AF31">
-        <v>0.0001246306087235887</v>
+        <v>0.000274423710208562</v>
       </c>
       <c r="AG31">
-        <v>0.0004514397604876657</v>
+        <v>0.0004028773617955485</v>
       </c>
       <c r="AH31">
-        <v>0.0008530272774858959</v>
+        <v>0.0008077009910393846</v>
       </c>
     </row>
     <row r="32" spans="1:34">
@@ -3708,13 +3708,13 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>2.769569082746416E-06</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="F32">
-        <v>2.769569082746416E-06</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -3732,43 +3732,43 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>1.384784541373208E-05</v>
+        <v>7.785069793150696E-06</v>
       </c>
       <c r="M32">
-        <v>0.0001661741449647849</v>
+        <v>5.644175600034255E-05</v>
       </c>
       <c r="N32">
-        <v>0.0001661741449647849</v>
+        <v>1.751640703458906E-05</v>
       </c>
       <c r="O32">
-        <v>0.0001357088850545744</v>
+        <v>5.838802344863021E-06</v>
       </c>
       <c r="P32">
-        <v>4.985224348943548E-05</v>
+        <v>1.167760468972604E-05</v>
       </c>
       <c r="Q32">
-        <v>2.769569082746416E-06</v>
+        <v>0</v>
       </c>
       <c r="R32">
-        <v>8.585664156513888E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="S32">
-        <v>6.370008890316756E-05</v>
+        <v>0</v>
       </c>
       <c r="T32">
-        <v>7.20087961514068E-05</v>
+        <v>3.892534896575348E-06</v>
       </c>
       <c r="U32">
-        <v>0.001600810929827428</v>
+        <v>0.003320332266778772</v>
       </c>
       <c r="V32">
         <v>0</v>
       </c>
       <c r="W32">
-        <v>3.877396715844982E-05</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="X32">
-        <v>1.938698357922491E-05</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="Y32">
         <v>0</v>
@@ -3777,7 +3777,7 @@
         <v>0</v>
       </c>
       <c r="AA32">
-        <v>0</v>
+        <v>9.73133724143837E-06</v>
       </c>
       <c r="AB32">
         <v>0</v>
@@ -3792,7 +3792,7 @@
         <v>0</v>
       </c>
       <c r="AF32">
-        <v>2.769569082746416E-06</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="AG32">
         <v>0</v>
@@ -3806,85 +3806,85 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>6.646965798591397E-05</v>
+        <v>6.228055834520557E-05</v>
       </c>
       <c r="C33">
-        <v>0.0003877396715844981</v>
+        <v>0.0005780414321414391</v>
       </c>
       <c r="D33">
-        <v>0.0002548003556126702</v>
+        <v>0.0003561669430366443</v>
       </c>
       <c r="E33">
-        <v>0.0001107827633098566</v>
+        <v>9.73133724143837E-05</v>
       </c>
       <c r="F33">
-        <v>0.0003905092406672446</v>
+        <v>0.0005410623506239734</v>
       </c>
       <c r="G33">
-        <v>2.215655266197132E-05</v>
+        <v>5.449548855205487E-05</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0.0001107827633098566</v>
+        <v>0.0001148297794489728</v>
       </c>
       <c r="J33">
-        <v>0.0002187959575369668</v>
+        <v>9.536710496609602E-05</v>
       </c>
       <c r="K33">
-        <v>0.0002215655266197132</v>
+        <v>0.0003561669430366443</v>
       </c>
       <c r="L33">
-        <v>1.938698357922491E-05</v>
+        <v>0</v>
       </c>
       <c r="M33">
-        <v>0.0003461961353433019</v>
+        <v>0.0002335520937945209</v>
       </c>
       <c r="N33">
-        <v>0.0001080131942271102</v>
+        <v>6.228055834520557E-05</v>
       </c>
       <c r="O33">
-        <v>0.0002049481121232348</v>
+        <v>0.0002101968844150688</v>
       </c>
       <c r="P33">
-        <v>0.0002298742338679525</v>
+        <v>0.0004048236292438362</v>
       </c>
       <c r="Q33">
-        <v>0.0001523262995510528</v>
+        <v>0.000190734209932192</v>
       </c>
       <c r="R33">
-        <v>0.0003185004445158378</v>
+        <v>0.0003347580011054799</v>
       </c>
       <c r="S33">
-        <v>0.0001966394048749955</v>
+        <v>0.0001557013958630139</v>
       </c>
       <c r="T33">
-        <v>0.0004043570860809766</v>
+        <v>0.0005605250251068501</v>
       </c>
       <c r="U33">
-        <v>0.0005456051093010438</v>
+        <v>0.0005099220714513705</v>
       </c>
       <c r="V33">
-        <v>3.60043980757034E-05</v>
+        <v>0.0001148297794489728</v>
       </c>
       <c r="W33">
-        <v>3.60043980757034E-05</v>
+        <v>6.228055834520557E-05</v>
       </c>
       <c r="X33">
-        <v>4.154353624119623E-05</v>
+        <v>1.557013958630139E-05</v>
       </c>
       <c r="Y33">
-        <v>8.308707248239247E-05</v>
+        <v>1.362387213801372E-05</v>
       </c>
       <c r="Z33">
-        <v>0.0002326438029506989</v>
+        <v>0.0003542206755883567</v>
       </c>
       <c r="AA33">
-        <v>6.370008890316756E-05</v>
+        <v>2.530147682773976E-05</v>
       </c>
       <c r="AB33">
-        <v>0.0005012920039771012</v>
+        <v>0.0002043580820702058</v>
       </c>
       <c r="AC33">
         <v>0</v>
@@ -3896,13 +3896,13 @@
         <v>0</v>
       </c>
       <c r="AF33">
-        <v>3.323482899295698E-05</v>
+        <v>5.254922110376719E-05</v>
       </c>
       <c r="AG33">
-        <v>4.154353624119623E-05</v>
+        <v>3.308654662089046E-05</v>
       </c>
       <c r="AH33">
-        <v>3.323482899295698E-05</v>
+        <v>9.925963986267137E-05</v>
       </c>
     </row>
     <row r="34" spans="1:34">
@@ -3910,85 +3910,85 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.0002187959575369668</v>
+        <v>0.0002179819542082195</v>
       </c>
       <c r="C34">
-        <v>0.0005151398493908332</v>
+        <v>0.0005663638274517131</v>
       </c>
       <c r="D34">
-        <v>0.001523262995510528</v>
+        <v>0.001996870401943153</v>
       </c>
       <c r="E34">
-        <v>0.0004791354513151299</v>
+        <v>0.0003970385594506855</v>
       </c>
       <c r="F34">
-        <v>0.0007948663267482212</v>
+        <v>0.001276751446076714</v>
       </c>
       <c r="G34">
-        <v>0.0003101917372675986</v>
+        <v>0.0005099220714513705</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0.000279726477357388</v>
+        <v>0.0003094565242777401</v>
       </c>
       <c r="J34">
-        <v>0.0005871486455422401</v>
+        <v>0.002779269916154798</v>
       </c>
       <c r="K34">
-        <v>0.0007256270996795609</v>
+        <v>0.001267020108835276</v>
       </c>
       <c r="L34">
-        <v>0.0001080131942271102</v>
+        <v>2.919401172431511E-05</v>
       </c>
       <c r="M34">
-        <v>0.0009278056427200491</v>
+        <v>0.0009964889335232891</v>
       </c>
       <c r="N34">
-        <v>0.00114383203117427</v>
+        <v>0.00117943807366233</v>
       </c>
       <c r="O34">
-        <v>0.0008114837412446997</v>
+        <v>0.0007746144444184942</v>
       </c>
       <c r="P34">
-        <v>0.002030094137653122</v>
+        <v>0.002354983612428085</v>
       </c>
       <c r="Q34">
-        <v>0.0005788399382940008</v>
+        <v>0.0008038084561428093</v>
       </c>
       <c r="R34">
-        <v>0.001201992981911944</v>
+        <v>0.00123004102731781</v>
       </c>
       <c r="S34">
-        <v>0.0005428355402182975</v>
+        <v>0.0002724774427602743</v>
       </c>
       <c r="T34">
-        <v>0.001598041360744682</v>
+        <v>0.001887879424839044</v>
       </c>
       <c r="U34">
-        <v>0.001938698357922491</v>
+        <v>0.002578804368981168</v>
       </c>
       <c r="V34">
-        <v>0.000246491648364431</v>
+        <v>0.0003892534896575348</v>
       </c>
       <c r="W34">
-        <v>6.646965798591397E-05</v>
+        <v>0.000268584907863699</v>
       </c>
       <c r="X34">
-        <v>0.0003295787208468234</v>
+        <v>0.0003289191987606169</v>
       </c>
       <c r="Y34">
-        <v>9.416534881337813E-05</v>
+        <v>0.0001206685817938358</v>
       </c>
       <c r="Z34">
-        <v>0.0003489657044260483</v>
+        <v>0.0006909249441421243</v>
       </c>
       <c r="AA34">
-        <v>0.0001218610396408423</v>
+        <v>5.254922110376719E-05</v>
       </c>
       <c r="AB34">
-        <v>0.0002631090628609095</v>
+        <v>0.0001751640703458907</v>
       </c>
       <c r="AC34">
         <v>0</v>
@@ -4000,13 +4000,13 @@
         <v>0</v>
       </c>
       <c r="AF34">
-        <v>7.754793431689964E-05</v>
+        <v>0.0001926804773804797</v>
       </c>
       <c r="AG34">
-        <v>0.0001274001778063351</v>
+        <v>0.0001615401982078769</v>
       </c>
       <c r="AH34">
-        <v>0.0001357088850545744</v>
+        <v>0.0003094565242777401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>